<commit_message>
First merge ok and improvements
</commit_message>
<xml_diff>
--- a/pp/tracesV2/AnalyseAlgoLevenshtein.xlsx
+++ b/pp/tracesV2/AnalyseAlgoLevenshtein.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10020" windowHeight="4380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId3"/>
+    <sheet name="Feuil4" sheetId="4" r:id="rId2"/>
+    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -212,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="115">
   <si>
     <t>v</t>
   </si>
@@ -2432,89 +2433,95 @@
     <t>*A[[*AB]C]</t>
   </si>
   <si>
-    <t>Principe : Action x- et tête de la pile son complément =&gt; chercher dans la pile le premier "x" ou "d", noté REF. Si on en trouve un, mettre tout ce qui est entre REF et la tête de la pile comme optionnel. Si on n'en trouve pas noter tous les prochains ajouts comme optionnel tant que cette tête de pile n'a pas été traitée (Attention il est possible que d'autres imbrications soient empilées par dessus, c'est donc vraiment cette action qui est visée). Retirer le x de la pile (ce n'est donc pas la tête).</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*ABC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*ABC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
+    <t>Principe : Action x- et tête de la pile son complément =&gt; chercher dans la pile le premier "x" ou "d", noté REF. Mettre tout ce qui est entre REF et la tête de la pile comme optionnel. Noter la tête de pile comme "altérée", tant que cette action altérée se trouve en tête de pile toute nouvelle insertion dans le vecteur de fusion sera noté optionnelle. Retirer le REF de la pile (ce n'est donc pas la tête) si REF est un d remplacer le d par le complément de x.</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A[*D*E]BC</t>
   </si>
 </sst>
 </file>
@@ -2624,7 +2631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2741,6 +2748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3023,7 +3031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI148"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
+    <sheetView topLeftCell="A77" workbookViewId="0">
       <selection activeCell="H145" sqref="H145"/>
     </sheetView>
   </sheetViews>
@@ -7215,6 +7223,277 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="40">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="40">
+        <v>0</v>
+      </c>
+      <c r="D12" s="40">
+        <v>1</v>
+      </c>
+      <c r="E12" s="40">
+        <v>2</v>
+      </c>
+      <c r="F12" s="40">
+        <v>3</v>
+      </c>
+      <c r="G12" s="40">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13" s="40">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI153"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
@@ -12002,11 +12281,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -12484,7 +12763,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F18" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -12908,7 +13187,7 @@
         <v>105</v>
       </c>
       <c r="K37" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>